<commit_message>
IceWind Dale - new equipment; CastleCLash - news skills
</commit_message>
<xml_diff>
--- a/CastleClash/heroes.xlsx
+++ b/CastleClash/heroes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="97">
   <si>
     <t>Name</t>
   </si>
@@ -208,25 +208,115 @@
     <t>Revive</t>
   </si>
   <si>
-    <t>Revive with X% HP restored</t>
-  </si>
-  <si>
     <t>Heavy blow</t>
   </si>
   <si>
-    <t>Has a X% chance to inflict coma for X sec on target when attacking</t>
-  </si>
-  <si>
     <t>Scorch</t>
   </si>
   <si>
-    <t>Has a X% chance to negate all damage when attacked</t>
-  </si>
-  <si>
     <t>Revitalize</t>
   </si>
   <si>
-    <t>Gain X% energy at the start of battle</t>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Increases mov spd by X %</t>
+  </si>
+  <si>
+    <t>Tenacity</t>
+  </si>
+  <si>
+    <t>Increases HP by X %</t>
+  </si>
+  <si>
+    <t>Flame guard</t>
+  </si>
+  <si>
+    <t>Deflects X% of damage taken</t>
+  </si>
+  <si>
+    <t>Deadly strike</t>
+  </si>
+  <si>
+    <t>Slow down</t>
+  </si>
+  <si>
+    <t>War god</t>
+  </si>
+  <si>
+    <t>Increases ATK by X %</t>
+  </si>
+  <si>
+    <t>Gain X % energy at the start of battle</t>
+  </si>
+  <si>
+    <t>Has a X % chance to negate all damage when attacked</t>
+  </si>
+  <si>
+    <t>Has a X % chance to inflict coma for X sec on target when attacking</t>
+  </si>
+  <si>
+    <t>Revive with X % HP restored</t>
+  </si>
+  <si>
+    <t>Life drain</t>
+  </si>
+  <si>
+    <t>Restores X % of HP with each attack</t>
+  </si>
+  <si>
+    <t>Stone skin</t>
+  </si>
+  <si>
+    <t>Reduces damage taken by X %</t>
+  </si>
+  <si>
+    <t>Berserk</t>
+  </si>
+  <si>
+    <t>Increases ATK SPD by X %</t>
+  </si>
+  <si>
+    <t>Self destruct</t>
+  </si>
+  <si>
+    <t>Deals X % damage to nearby enemies upon death</t>
+  </si>
+  <si>
+    <t>Scatter</t>
+  </si>
+  <si>
+    <t>Reduces targets energy by X when attacking</t>
+  </si>
+  <si>
+    <t>Restores the HP of X nearby allies with the lowest HP by X % ATK and increases their ATK by X % for X secs</t>
+  </si>
+  <si>
+    <t>Blade shell</t>
+  </si>
+  <si>
+    <t>Has a X % chance to deflect X % of damage taken</t>
+  </si>
+  <si>
+    <t>Has a X % chance to steal X more damage when attacking</t>
+  </si>
+  <si>
+    <t>Has a X % chance to reduce enemy SPD by X % for X secs when attacking</t>
+  </si>
+  <si>
+    <t>All enemy healing effects are reduced by X % for X secs</t>
+  </si>
+  <si>
+    <t>Deals X % damage to target, inflicting coma for X secs</t>
+  </si>
+  <si>
+    <t>Invisible: deflects DMG from all sources except buildings for X secs (cooldown required)</t>
+  </si>
+  <si>
+    <t>Deals X % DMG to target</t>
+  </si>
+  <si>
+    <t>Surrounds Immortep within a sandstorm for X secs. Has a chance to deal X %</t>
   </si>
 </sst>
 </file>
@@ -949,17 +1039,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{080C996C-4A0B-4B5B-A051-BA1CF7631A38}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="69.88671875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="87.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -971,35 +1061,179 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="B5" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B6" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>